<commit_message>
removes speed column from instantaneous data table and validates xml
</commit_message>
<xml_diff>
--- a/data-raw/metadata/yuba_instantaneous_passage.xlsx
+++ b/data-raw/metadata/yuba_instantaneous_passage.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10414"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/liz/Documents/code/SRJPE/EDI/jpe-yuba-adult-edi/data-raw/metadata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68EEEAA9-8AD3-BE44-B560-07A9802D341D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FDC43A6-DCA4-AC44-B902-F3E88AC66865}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20380" yWindow="-26620" windowWidth="30240" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1140" yWindow="2620" windowWidth="30240" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="attribute" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="51">
   <si>
     <t xml:space="preserve">attribute_name </t>
   </si>
@@ -115,9 +115,6 @@
     <t>direction_of_passage</t>
   </si>
   <si>
-    <t>speed</t>
-  </si>
-  <si>
     <t>species</t>
   </si>
   <si>
@@ -137,9 +134,6 @@
   </si>
   <si>
     <t xml:space="preserve">Direction of fish travel through VAKI chute. Levels = c("up", "down"). </t>
-  </si>
-  <si>
-    <t>Speed of fish travel through VAKI chute, as estimated by VAKI Winari software.</t>
   </si>
   <si>
     <t>Whether or not fish observed had a clipped adipose fin, determined by PSMFC staff review of VAKI imagery. Levels = c("TRUE", "FALSE", "undetermined").</t>
@@ -179,9 +173,6 @@
   </si>
   <si>
     <t>yuba_instantaneous_passage</t>
-  </si>
-  <si>
-    <t>metersPerSecond</t>
   </si>
   <si>
     <t>00:00:00</t>
@@ -263,7 +254,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -292,8 +283,6 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="4" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -509,11 +498,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z996"/>
+  <dimension ref="A1:Z995"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="147" zoomScaleNormal="147" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="147" zoomScaleNormal="147" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L9" sqref="L9"/>
+      <selection pane="bottomLeft" activeCell="A8" sqref="A8:XFD8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -593,13 +582,13 @@
         <v>23</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>16</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="E2" s="4" t="s">
         <v>16</v>
@@ -613,10 +602,10 @@
       </c>
       <c r="K2" s="5"/>
       <c r="L2" s="10" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="M2" s="10" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="N2" s="7"/>
       <c r="O2" s="7"/>
@@ -637,13 +626,13 @@
         <v>24</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>16</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="E3" s="4" t="s">
         <v>16</v>
@@ -653,14 +642,14 @@
       <c r="H3" s="6"/>
       <c r="I3" s="5"/>
       <c r="J3" s="6" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="K3" s="5"/>
       <c r="L3" s="10" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="M3" s="10" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="N3" s="7"/>
       <c r="O3" s="7"/>
@@ -681,13 +670,13 @@
         <v>25</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>14</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="E4" s="4" t="s">
         <v>15</v>
@@ -696,10 +685,10 @@
         <v>14</v>
       </c>
       <c r="G4" s="6" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="H4" s="6" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="I4" s="5"/>
       <c r="J4" s="6"/>
@@ -729,13 +718,13 @@
         <v>26</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>14</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="E5" s="4" t="s">
         <v>15</v>
@@ -744,18 +733,18 @@
         <v>14</v>
       </c>
       <c r="G5" s="6" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="H5" s="6" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="I5" s="5"/>
       <c r="J5" s="6"/>
       <c r="K5" s="5"/>
-      <c r="L5" s="17">
+      <c r="L5" s="6">
         <v>0</v>
       </c>
-      <c r="M5" s="17">
+      <c r="M5" s="6">
         <v>189</v>
       </c>
       <c r="N5" s="7"/>
@@ -777,13 +766,13 @@
         <v>27</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C6" s="4" t="s">
         <v>22</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="E6" s="4" t="s">
         <v>13</v>
@@ -815,13 +804,13 @@
         <v>28</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C7" s="4" t="s">
         <v>22</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="E7" s="4" t="s">
         <v>13</v>
@@ -850,38 +839,28 @@
     </row>
     <row r="8" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
-      <c r="F8" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="G8" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="H8" s="6" t="s">
-        <v>42</v>
-      </c>
+      <c r="F8" s="6"/>
+      <c r="G8" s="6"/>
+      <c r="H8" s="6"/>
       <c r="I8" s="5"/>
       <c r="J8" s="6"/>
       <c r="K8" s="5"/>
-      <c r="L8" s="16">
-        <v>-2.61</v>
-      </c>
-      <c r="M8" s="6">
-        <v>5.71</v>
-      </c>
+      <c r="L8" s="13"/>
+      <c r="M8" s="6"/>
       <c r="N8" s="7"/>
       <c r="O8" s="7"/>
       <c r="P8" s="7"/>
@@ -898,16 +877,16 @@
     </row>
     <row r="9" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
-        <v>21</v>
+        <v>29</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C9" s="4" t="s">
         <v>22</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="E9" s="4" t="s">
         <v>13</v>
@@ -918,8 +897,8 @@
       <c r="I9" s="5"/>
       <c r="J9" s="6"/>
       <c r="K9" s="5"/>
-      <c r="L9" s="13"/>
-      <c r="M9" s="6"/>
+      <c r="L9" s="12"/>
+      <c r="M9" s="12"/>
       <c r="N9" s="7"/>
       <c r="O9" s="7"/>
       <c r="P9" s="7"/>
@@ -936,28 +915,38 @@
     </row>
     <row r="10" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
-        <v>30</v>
+        <v>44</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
-      <c r="F10" s="6"/>
-      <c r="G10" s="6"/>
-      <c r="H10" s="6"/>
+      <c r="F10" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="G10" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="H10" s="6" t="s">
+        <v>47</v>
+      </c>
       <c r="I10" s="5"/>
       <c r="J10" s="6"/>
       <c r="K10" s="5"/>
-      <c r="L10" s="12"/>
-      <c r="M10" s="12"/>
+      <c r="L10" s="12">
+        <v>1</v>
+      </c>
+      <c r="M10" s="6">
+        <v>1</v>
+      </c>
       <c r="N10" s="7"/>
       <c r="O10" s="7"/>
       <c r="P10" s="7"/>
@@ -973,39 +962,19 @@
       <c r="Z10" s="7"/>
     </row>
     <row r="11" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="B11" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="C11" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="D11" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="E11" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="F11" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="G11" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="H11" s="6" t="s">
-        <v>49</v>
-      </c>
+      <c r="A11" s="4"/>
+      <c r="B11" s="4"/>
+      <c r="C11" s="4"/>
+      <c r="D11" s="5"/>
+      <c r="E11" s="4"/>
+      <c r="F11" s="6"/>
+      <c r="G11" s="6"/>
+      <c r="H11" s="6"/>
       <c r="I11" s="5"/>
       <c r="J11" s="6"/>
       <c r="K11" s="5"/>
-      <c r="L11" s="12">
-        <v>1</v>
-      </c>
-      <c r="M11" s="6">
-        <v>1</v>
-      </c>
+      <c r="L11" s="12"/>
+      <c r="M11" s="6"/>
       <c r="N11" s="7"/>
       <c r="O11" s="7"/>
       <c r="P11" s="7"/>
@@ -1032,7 +1001,7 @@
       <c r="I12" s="5"/>
       <c r="J12" s="6"/>
       <c r="K12" s="5"/>
-      <c r="L12" s="12"/>
+      <c r="L12" s="13"/>
       <c r="M12" s="6"/>
       <c r="N12" s="7"/>
       <c r="O12" s="7"/>
@@ -1050,18 +1019,18 @@
     </row>
     <row r="13" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="4"/>
-      <c r="B13" s="4"/>
-      <c r="C13" s="4"/>
-      <c r="D13" s="5"/>
-      <c r="E13" s="4"/>
-      <c r="F13" s="6"/>
-      <c r="G13" s="6"/>
-      <c r="H13" s="6"/>
-      <c r="I13" s="5"/>
-      <c r="J13" s="6"/>
-      <c r="K13" s="5"/>
-      <c r="L13" s="13"/>
-      <c r="M13" s="6"/>
+      <c r="B13" s="7"/>
+      <c r="C13" s="7"/>
+      <c r="D13" s="14"/>
+      <c r="E13" s="7"/>
+      <c r="F13" s="15"/>
+      <c r="G13" s="15"/>
+      <c r="H13" s="15"/>
+      <c r="I13" s="14"/>
+      <c r="J13" s="15"/>
+      <c r="K13" s="14"/>
+      <c r="L13" s="15"/>
+      <c r="M13" s="15"/>
       <c r="N13" s="7"/>
       <c r="O13" s="7"/>
       <c r="P13" s="7"/>
@@ -1160,9 +1129,8 @@
       <c r="Y16" s="7"/>
       <c r="Z16" s="7"/>
     </row>
-    <row r="17" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:26" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="4"/>
-      <c r="B17" s="7"/>
       <c r="C17" s="7"/>
       <c r="D17" s="14"/>
       <c r="E17" s="7"/>
@@ -1188,8 +1156,9 @@
       <c r="Y17" s="7"/>
       <c r="Z17" s="7"/>
     </row>
-    <row r="18" spans="1:26" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="4"/>
+      <c r="B18" s="7"/>
       <c r="C18" s="7"/>
       <c r="D18" s="14"/>
       <c r="E18" s="7"/>
@@ -1357,34 +1326,34 @@
     </row>
     <row r="24" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="4"/>
-      <c r="B24" s="7"/>
       <c r="C24" s="7"/>
       <c r="D24" s="14"/>
       <c r="E24" s="7"/>
-      <c r="F24" s="15"/>
-      <c r="G24" s="15"/>
-      <c r="H24" s="15"/>
-      <c r="I24" s="14"/>
-      <c r="J24" s="15"/>
-      <c r="K24" s="14"/>
-      <c r="L24" s="15"/>
-      <c r="M24" s="15"/>
-      <c r="N24" s="7"/>
-      <c r="O24" s="7"/>
-      <c r="P24" s="7"/>
-      <c r="Q24" s="7"/>
-      <c r="R24" s="7"/>
-      <c r="S24" s="7"/>
-      <c r="T24" s="7"/>
-      <c r="U24" s="7"/>
-      <c r="V24" s="7"/>
-      <c r="W24" s="7"/>
-      <c r="X24" s="7"/>
-      <c r="Y24" s="7"/>
-      <c r="Z24" s="7"/>
+      <c r="F24" s="6"/>
+      <c r="G24" s="6"/>
+      <c r="H24" s="6"/>
+      <c r="I24" s="5"/>
+      <c r="J24" s="6"/>
+      <c r="K24" s="5"/>
+      <c r="L24" s="6"/>
+      <c r="M24" s="6"/>
+      <c r="N24" s="4"/>
+      <c r="O24" s="4"/>
+      <c r="P24" s="4"/>
+      <c r="Q24" s="4"/>
+      <c r="R24" s="4"/>
+      <c r="S24" s="4"/>
+      <c r="T24" s="4"/>
+      <c r="U24" s="4"/>
+      <c r="V24" s="4"/>
+      <c r="W24" s="4"/>
+      <c r="X24" s="4"/>
+      <c r="Y24" s="4"/>
+      <c r="Z24" s="4"/>
     </row>
     <row r="25" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="4"/>
+      <c r="B25" s="7"/>
       <c r="C25" s="7"/>
       <c r="D25" s="14"/>
       <c r="E25" s="7"/>
@@ -1416,39 +1385,29 @@
       <c r="C26" s="7"/>
       <c r="D26" s="14"/>
       <c r="E26" s="7"/>
-      <c r="F26" s="6"/>
-      <c r="G26" s="6"/>
-      <c r="H26" s="6"/>
-      <c r="I26" s="5"/>
-      <c r="J26" s="6"/>
-      <c r="K26" s="5"/>
-      <c r="L26" s="6"/>
-      <c r="M26" s="6"/>
-      <c r="N26" s="4"/>
-      <c r="O26" s="4"/>
-      <c r="P26" s="4"/>
-      <c r="Q26" s="4"/>
-      <c r="R26" s="4"/>
-      <c r="S26" s="4"/>
-      <c r="T26" s="4"/>
-      <c r="U26" s="4"/>
-      <c r="V26" s="4"/>
-      <c r="W26" s="4"/>
-      <c r="X26" s="4"/>
-      <c r="Y26" s="4"/>
-      <c r="Z26" s="4"/>
+      <c r="F26" s="15"/>
+      <c r="G26" s="15"/>
+      <c r="H26" s="15"/>
+      <c r="I26" s="14"/>
+      <c r="J26" s="15"/>
+      <c r="K26" s="14"/>
+      <c r="L26" s="15"/>
+      <c r="M26" s="15"/>
+      <c r="N26" s="7"/>
+      <c r="O26" s="7"/>
+      <c r="P26" s="7"/>
+      <c r="Q26" s="7"/>
+      <c r="R26" s="7"/>
+      <c r="S26" s="7"/>
+      <c r="T26" s="7"/>
+      <c r="U26" s="7"/>
+      <c r="V26" s="7"/>
+      <c r="W26" s="7"/>
+      <c r="X26" s="7"/>
+      <c r="Y26" s="7"/>
+      <c r="Z26" s="7"/>
     </row>
     <row r="27" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="4"/>
-      <c r="B27" s="7"/>
-      <c r="C27" s="7"/>
-      <c r="D27" s="14"/>
-      <c r="E27" s="7"/>
-      <c r="F27" s="15"/>
-      <c r="G27" s="15"/>
-      <c r="H27" s="15"/>
-      <c r="I27" s="14"/>
-      <c r="J27" s="15"/>
       <c r="K27" s="14"/>
       <c r="L27" s="15"/>
       <c r="M27" s="15"/>
@@ -1467,6 +1426,16 @@
       <c r="Z27" s="7"/>
     </row>
     <row r="28" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="4"/>
+      <c r="B28" s="7"/>
+      <c r="C28" s="7"/>
+      <c r="D28" s="14"/>
+      <c r="E28" s="7"/>
+      <c r="F28" s="15"/>
+      <c r="G28" s="15"/>
+      <c r="H28" s="15"/>
+      <c r="I28" s="14"/>
+      <c r="J28" s="15"/>
       <c r="K28" s="14"/>
       <c r="L28" s="15"/>
       <c r="M28" s="15"/>
@@ -1597,7 +1566,6 @@
       <c r="Z32" s="7"/>
     </row>
     <row r="33" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="4"/>
       <c r="B33" s="7"/>
       <c r="C33" s="7"/>
       <c r="D33" s="14"/>
@@ -1625,6 +1593,7 @@
       <c r="Z33" s="7"/>
     </row>
     <row r="34" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A34" s="4"/>
       <c r="B34" s="7"/>
       <c r="C34" s="7"/>
       <c r="D34" s="14"/>
@@ -1652,7 +1621,6 @@
       <c r="Z34" s="7"/>
     </row>
     <row r="35" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="4"/>
       <c r="B35" s="7"/>
       <c r="C35" s="7"/>
       <c r="D35" s="14"/>
@@ -1680,6 +1648,7 @@
       <c r="Z35" s="7"/>
     </row>
     <row r="36" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A36" s="4"/>
       <c r="B36" s="7"/>
       <c r="C36" s="7"/>
       <c r="D36" s="14"/>
@@ -2631,7 +2600,7 @@
       <c r="Z69" s="7"/>
     </row>
     <row r="70" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A70" s="4"/>
+      <c r="A70" s="7"/>
       <c r="B70" s="7"/>
       <c r="C70" s="7"/>
       <c r="D70" s="14"/>
@@ -28558,46 +28527,18 @@
       <c r="Y995" s="7"/>
       <c r="Z995" s="7"/>
     </row>
-    <row r="996" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A996" s="7"/>
-      <c r="B996" s="7"/>
-      <c r="C996" s="7"/>
-      <c r="D996" s="14"/>
-      <c r="E996" s="7"/>
-      <c r="F996" s="15"/>
-      <c r="G996" s="15"/>
-      <c r="H996" s="15"/>
-      <c r="I996" s="14"/>
-      <c r="J996" s="15"/>
-      <c r="K996" s="14"/>
-      <c r="L996" s="15"/>
-      <c r="M996" s="15"/>
-      <c r="N996" s="7"/>
-      <c r="O996" s="7"/>
-      <c r="P996" s="7"/>
-      <c r="Q996" s="7"/>
-      <c r="R996" s="7"/>
-      <c r="S996" s="7"/>
-      <c r="T996" s="7"/>
-      <c r="U996" s="7"/>
-      <c r="V996" s="7"/>
-      <c r="W996" s="7"/>
-      <c r="X996" s="7"/>
-      <c r="Y996" s="7"/>
-      <c r="Z996" s="7"/>
-    </row>
   </sheetData>
   <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="C53:C996 C29:C41 C1:C27" xr:uid="{00000000-0002-0000-0000-000002000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="C52:C995 C28:C40 C1:C26" xr:uid="{00000000-0002-0000-0000-000002000000}">
       <formula1>"nominal,ordinal,interval,ratio,dateTime"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="E29:E996 E1:E27" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="E28:E995 E1:E26" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"text,enumerated,dateTime,numeric"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="F29:F996 F1:F27" xr:uid="{00000000-0002-0000-0000-000001000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="F28:F995 F1:F26" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>"ratio,interval"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="H29:H996 H1:H27" xr:uid="{00000000-0002-0000-0000-000003000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="H28:H995 H1:H26" xr:uid="{00000000-0002-0000-0000-000003000000}">
       <formula1>"natural,whole,integer,real"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>